<commit_message>
Adding banner on main page
</commit_message>
<xml_diff>
--- a/bumagia_data.xlsx
+++ b/bumagia_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="525" windowWidth="23655" windowHeight="13995" tabRatio="687"/>
+    <workbookView xWindow="150" yWindow="525" windowWidth="23655" windowHeight="13995" tabRatio="687" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="common_data" sheetId="3" r:id="rId1"/>
@@ -895,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2339,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2359,7 +2359,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="A9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>16</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1">
       <c r="A14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1">
       <c r="A18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>29</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>33</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>34</v>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>10</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>21</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>35</v>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1">
       <c r="A38" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Link to updated catalog added
</commit_message>
<xml_diff>
--- a/bumagia_data.xlsx
+++ b/bumagia_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="525" windowWidth="23655" windowHeight="13995" tabRatio="687"/>
+    <workbookView xWindow="150" yWindow="525" windowWidth="23655" windowHeight="13995" tabRatio="687" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="common_data" sheetId="3" r:id="rId1"/>
@@ -500,9 +500,6 @@
     <t>Что использовали для наполнения коробок для посылок раньше? Мятую газету? Пупырчатую пленку? Пришло время новых решений — экономичных и экологичных! Экофиллер — новый материал для использования в упаковке надежно сохранит содержимое коробки, а своей яркостью и необычностью подарит адресату незабываемые эмоции. Узнайте больше о нашей новой линейке бумажного экофиллера и выберите для себя тот, который наилучшим образом подходит именно вам!</t>
   </si>
   <si>
-    <t>Мятая газета или неэкологичная синтетическая пузырьковая пленка для использования в упаковке? Вчерашний день! Сегодня в моде экофиллер — новый материал, который не только сохранит в полной безопасности содержимое, но и своим ярким и необычным внешним видом подарит адресату вашей посылки незабываемые эмоции. Превратить обычный подарок в волшебный сюрприз? Легко! Добавьте в упаковку немного цветного экофиллера, и ощущение праздника  возникнет тут же, как только коробка будет открыта! Широкая цветовая гамма и бескомпромиссное качество изготовления нашего экофиллера характеризуют его как продукт, способный заменить давно устаревшие материалы для использования в упаковке и презентации ваших товаров.</t>
-  </si>
-  <si>
     <t>bumagia.com.ua | экофиллер</t>
   </si>
   <si>
@@ -549,6 +546,9 @@
   </si>
   <si>
     <t>Время не стоит на месте, и многие привычные вещи, еще вчера считавшиеся вполне приемлемыми, сегодня безнадёжно устарели. Чем заполняли коробки для посылок вчера, чтобы хрупкое или ценное содержимое не пострадало при транспортировке? Мятой газетой или оберточной бумагой, в лучшем случае — воздушно-пузырьковой пленкой. Но если вам не все равно, в каком виде предстанет ваше отправление адресату, если вам хочется удивить его заботой и вниманием, подарить радостные эмоции от распаковки подарка, то самое время обратить внимание на наш новый оригинальный продукт.&lt;/p&gt;&lt;p&gt;&lt;a href="http://ecofiller.com.ua"&gt;Экофиллер&lt;/a&gt; представляет собой множество аккуратно и точно нарезанных бумажых полосок шириной 2 мм. Благодаря специальной технологии смешивания, они образуют отличную упругую массу, которая не испортит своим внешним видом содержимое вашей посылки и при этом обладает прекрасными амортизирующими свойствами. Широкая цветовая гамма не оставит равнодушным никого, а экономичность использования (так, на коробку объемным весом 1 кг достаточно всего половины стандартной пачки (50 г) экофиллера) делает этот продукт поистине уникальным.</t>
+  </si>
+  <si>
+    <t>Мятая газета или неэкологичная синтетическая пузырьковая пленка для использования в упаковке? Вчерашний день! Сегодня в моде &lt;a href="products/ecofiller.html"&gt;экофиллер&lt;/a&gt; — новый материал, который не только сохранит в полной безопасности содержимое, но и своим ярким и необычным внешним видом подарит адресату вашей посылки незабываемые эмоции. Превратить обычный подарок в волшебный сюрприз? Легко! Добавьте в упаковку немного цветного экофиллера, и ощущение праздника  возникнет тут же, как только коробка будет открыта! Широкая цветовая гамма и бескомпромиссное качество изготовления нашего экофиллера характеризуют его как продукт, способный заменить давно устаревшие материалы для использования в упаковке и презентации ваших товаров.</t>
   </si>
 </sst>
 </file>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1047,7 +1047,7 @@
         <v>76</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="29.25" customHeight="1">
@@ -1055,15 +1055,15 @@
         <v>77</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
@@ -1344,7 +1344,7 @@
         <v>155</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1358,10 +1358,10 @@
     </row>
     <row r="17" spans="1:11" s="19" customFormat="1" ht="249.75" customHeight="1">
       <c r="A17" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -2387,8 +2387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2562,7 +2562,7 @@
         <v>«Соняшник» • EF-7637</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G7"/>
     </row>
@@ -2700,7 +2700,7 @@
         <v>«Бузок» • EF-7699</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G13"/>
     </row>
@@ -2801,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="3">
         <v>4820090867743</v>
@@ -2884,7 +2884,7 @@
         <v>«Кобальт» • EF-7774</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21"/>
     </row>
@@ -2953,7 +2953,7 @@
         <v>«Гірчиця» • EF-7804</v>
       </c>
       <c r="F24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G24"/>
     </row>
@@ -3022,7 +3022,7 @@
         <v>«Салат» • EF-7835</v>
       </c>
       <c r="F27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G27"/>
     </row>
@@ -3045,7 +3045,7 @@
         <v>«Золота осінь» • EF-7842</v>
       </c>
       <c r="F28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G28"/>
     </row>
@@ -3229,7 +3229,7 @@
         <v>«Блакить» • EF-7927</v>
       </c>
       <c r="F36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G36"/>
     </row>
@@ -3252,7 +3252,7 @@
         <v>«Блакитна мрія» • EF-7934</v>
       </c>
       <c r="F37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G37"/>
     </row>
@@ -3298,7 +3298,7 @@
         <v>«Білий сніг» • EF-7958</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G39"/>
     </row>

</xml_diff>

<commit_message>
Bookmark template updated, item added
</commit_message>
<xml_diff>
--- a/bumagia_data.xlsx
+++ b/bumagia_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="525" windowWidth="23655" windowHeight="13995" tabRatio="687" activeTab="6"/>
+    <workbookView xWindow="150" yWindow="525" windowWidth="23655" windowHeight="13995" tabRatio="687" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="common_data" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="219">
   <si>
     <t>Шампань</t>
   </si>
@@ -567,13 +567,127 @@
   </si>
   <si>
     <t>«Ассорти», 20 цветов</t>
+  </si>
+  <si>
+    <t>Кошки</t>
+  </si>
+  <si>
+    <t>Собаки</t>
+  </si>
+  <si>
+    <t>Цветы</t>
+  </si>
+  <si>
+    <t>Спорт</t>
+  </si>
+  <si>
+    <t>Транспорт</t>
+  </si>
+  <si>
+    <t>Профессии</t>
+  </si>
+  <si>
+    <t>Девушки Европы</t>
+  </si>
+  <si>
+    <t>Стильные девушки</t>
+  </si>
+  <si>
+    <t>Классики украинской литературы</t>
+  </si>
+  <si>
+    <t>Раскраски-антистресс. Серия 2</t>
+  </si>
+  <si>
+    <t>Раскраски-антистресс. Серия 3</t>
+  </si>
+  <si>
+    <t>Животные в технике оригами</t>
+  </si>
+  <si>
+    <t>Орнаменты</t>
+  </si>
+  <si>
+    <t>Поделки из квиллинга</t>
+  </si>
+  <si>
+    <t>Поп-арт</t>
+  </si>
+  <si>
+    <t>Раскраски-антистресс</t>
+  </si>
+  <si>
+    <t>Модные футболки</t>
+  </si>
+  <si>
+    <t>Уличная культура</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-1154-koshki</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-1161-sobaki</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-1130-tsvety</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4902-sport</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-1123-transport</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-2014-professii</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4889-stilnye-devushki</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4865-klassiki-ukrainskoj-literatury</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-6180-antistress-2</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-6197-antistress-3</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-3905-zhivotnye-origami</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-3912-ornamenty</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4612-podelki-iz-kvillinga</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4681-pop-art</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4698-raskraska-antistress</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4704-modnye-futbolki</t>
+  </si>
+  <si>
+    <t>jpg</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4896-ulichnaya-kultura</t>
+  </si>
+  <si>
+    <t>http://www.bumagiy.com/products/zakladki-dlya-knig-kartonnye-8-sht-v-nabore-bm-4858-devushki-evropy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -627,6 +741,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -679,7 +801,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -752,6 +874,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -963,7 +1090,7 @@
   <dimension ref="A1:L1007"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -993,10 +1120,10 @@
         <v>0</v>
       </c>
       <c r="F1" s="10">
+        <v>1</v>
+      </c>
+      <c r="G1" s="10">
         <v>0</v>
-      </c>
-      <c r="G1" s="10">
-        <v>1</v>
       </c>
       <c r="H1" s="10">
         <v>0</v>
@@ -2407,7 +2534,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4386,13 +4513,420 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="6" max="6" width="107.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="22">
+        <v>4820090864896</v>
+      </c>
+      <c r="D1" s="31" t="str">
+        <f>CONCATENATE("BM-",RIGHT(C1,4))</f>
+        <v>BM-4896</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="22">
+        <v>4820090861154</v>
+      </c>
+      <c r="D2" s="31" t="str">
+        <f t="shared" ref="D2:D18" si="0">CONCATENATE("BM-",RIGHT(C2,4))</f>
+        <v>BM-1154</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="22">
+        <v>4820090861161</v>
+      </c>
+      <c r="D3" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-1161</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="22">
+        <v>4820090861130</v>
+      </c>
+      <c r="D4" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-1130</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="22">
+        <v>4820090864902</v>
+      </c>
+      <c r="D5" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-4902</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="22">
+        <v>4820090861123</v>
+      </c>
+      <c r="D6" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-1123</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="22">
+        <v>4820090862014</v>
+      </c>
+      <c r="D7" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-2014</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="22">
+        <v>4820090864858</v>
+      </c>
+      <c r="D8" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-4858</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="22">
+        <v>4820090864889</v>
+      </c>
+      <c r="D9" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-4889</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="22">
+        <v>4820090864865</v>
+      </c>
+      <c r="D10" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-4865</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="22">
+        <v>4820090864698</v>
+      </c>
+      <c r="D11" s="31" t="str">
+        <f>CONCATENATE("BM-",RIGHT(C11,4))</f>
+        <v>BM-4698</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="22">
+        <v>4820090866180</v>
+      </c>
+      <c r="D12" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-6180</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="22">
+        <v>4820090866197</v>
+      </c>
+      <c r="D13" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-6197</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="22">
+        <v>4820090864704</v>
+      </c>
+      <c r="D14" s="31" t="str">
+        <f>CONCATENATE("BM-",RIGHT(C14,4))</f>
+        <v>BM-4704</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="22">
+        <v>4820090864681</v>
+      </c>
+      <c r="D15" s="31" t="str">
+        <f>CONCATENATE("BM-",RIGHT(C15,4))</f>
+        <v>BM-4681</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" s="22">
+        <v>4820090863905</v>
+      </c>
+      <c r="D16" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-3905</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="22">
+        <v>4820090863912</v>
+      </c>
+      <c r="D17" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-3912</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="22">
+        <v>4820090864612</v>
+      </c>
+      <c r="D18" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>BM-4612</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F12" r:id="rId10"/>
+    <hyperlink ref="F13" r:id="rId11"/>
+    <hyperlink ref="F16" r:id="rId12"/>
+    <hyperlink ref="F17" r:id="rId13"/>
+    <hyperlink ref="F18" r:id="rId14"/>
+    <hyperlink ref="F15" r:id="rId15"/>
+    <hyperlink ref="F11" r:id="rId16"/>
+    <hyperlink ref="F14" r:id="rId17"/>
+    <hyperlink ref="F1" r:id="rId18"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="2400" verticalDpi="2400" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -4400,7 +4934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>